<commit_message>
removed prefilled data from the template
</commit_message>
<xml_diff>
--- a/src/main/resources/timesheet-template.xlsx
+++ b/src/main/resources/timesheet-template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalData\work\timesheet\wip\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\hhmmss\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D642AC96-7079-4AD8-A677-94875737ECEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13740"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Timesheet!$A$1:$I$51</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Day</t>
   </si>
@@ -152,35 +153,11 @@
   <si>
     <t>PO:</t>
   </si>
-  <si>
-    <t>2025-09</t>
-  </si>
-  <si>
-    <t>01.10.2025</t>
-  </si>
-  <si>
-    <t>work</t>
-  </si>
-  <si>
-    <t>po_no</t>
-  </si>
-  <si>
-    <t>My</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>my_profile</t>
-  </si>
-  <si>
-    <t>contract_no</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -263,7 +240,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,18 +250,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="52"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -404,7 +369,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -416,10 +381,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -428,11 +393,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -440,65 +401,59 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -514,9 +469,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -554,9 +509,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -591,7 +546,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -626,7 +581,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -799,14 +754,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -819,42 +774,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="D3" s="20" t="s">
+      <c r="B3" s="15"/>
+      <c r="D3" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="21" t="s">
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>27</v>
-      </c>
+      <c r="H3" s="9"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -863,76 +816,46 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="11"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="11"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:9" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
@@ -972,489 +895,401 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="18">
+      <c r="B13" s="30">
         <v>1</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="14"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="31">
+        <v>2</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="31">
+        <v>3</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="31">
+        <v>4</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+    </row>
+    <row r="17" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="31">
+        <v>5</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+    </row>
+    <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="31">
+        <v>6</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+    </row>
+    <row r="19" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="31">
+        <v>7</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+    </row>
+    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="31">
+        <v>8</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+    </row>
+    <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="31">
+        <v>9</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+    </row>
+    <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="31">
+        <v>10</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+    </row>
+    <row r="23" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="31">
+        <v>11</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+    </row>
+    <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="31">
+        <v>12</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+    </row>
+    <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="31">
+        <v>13</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+    </row>
+    <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="31">
+        <v>14</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+    </row>
+    <row r="27" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="31">
+        <v>15</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+    </row>
+    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="31">
+        <v>16</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="31">
+        <v>17</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+    </row>
+    <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="31">
+        <v>18</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+    </row>
+    <row r="31" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="31">
+        <v>19</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+    </row>
+    <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="31">
+        <v>20</v>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+    </row>
+    <row r="33" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="31">
+        <v>21</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+    </row>
+    <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="31">
+        <v>22</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+    </row>
+    <row r="35" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="31">
+        <v>23</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+    </row>
+    <row r="36" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="31">
+        <v>24</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+    </row>
+    <row r="37" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="31">
+        <v>25</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+    </row>
+    <row r="38" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="31">
         <v>26</v>
       </c>
-      <c r="D13" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="15">
-        <v>2</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15">
-        <v>3</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="15">
+      <c r="C38" s="14"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+    </row>
+    <row r="39" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="31">
+        <v>27</v>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+    </row>
+    <row r="40" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="31">
+        <v>28</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+    </row>
+    <row r="41" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="31">
+        <v>29</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+    </row>
+    <row r="42" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="31">
+        <v>30</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+    </row>
+    <row r="43" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="31"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+    </row>
+    <row r="44" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="11"/>
+      <c r="C44" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-    </row>
-    <row r="17" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="25">
-        <v>5</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-    </row>
-    <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="26">
-        <v>6</v>
-      </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-    </row>
-    <row r="19" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="26">
-        <v>7</v>
-      </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-    </row>
-    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="15">
-        <v>8</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-    </row>
-    <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="15">
-        <v>9</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-    </row>
-    <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="15">
-        <v>10</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-    </row>
-    <row r="23" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="15">
-        <v>11</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
-    </row>
-    <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="15">
-        <v>12</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="23">
-        <v>5</v>
-      </c>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-    </row>
-    <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="26">
-        <v>13</v>
-      </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-    </row>
-    <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="26">
-        <v>14</v>
-      </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-    </row>
-    <row r="27" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="15">
-        <v>15</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-    </row>
-    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="15">
-        <v>16</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-    </row>
-    <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="15">
-        <v>17</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
-    </row>
-    <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="15">
-        <v>18</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-    </row>
-    <row r="31" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="15">
-        <v>19</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" s="23">
-        <v>5</v>
-      </c>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-    </row>
-    <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="26">
-        <v>20</v>
-      </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
-    </row>
-    <row r="33" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="26">
-        <v>21</v>
-      </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-    </row>
-    <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="15">
-        <v>22</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-    </row>
-    <row r="35" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="15">
-        <v>23</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D35" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-    </row>
-    <row r="36" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="15">
-        <v>24</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
-    </row>
-    <row r="37" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="15">
-        <v>25</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D37" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-    </row>
-    <row r="38" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="15">
-        <v>26</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38" s="23">
-        <v>5</v>
-      </c>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
-    </row>
-    <row r="39" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="26">
-        <v>27</v>
-      </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-    </row>
-    <row r="40" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="26">
-        <v>28</v>
-      </c>
-      <c r="C40" s="16"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-    </row>
-    <row r="41" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="15">
-        <v>29</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D41" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
-    </row>
-    <row r="42" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="15">
-        <v>30</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D42" s="23">
-        <v>8.5</v>
-      </c>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="24"/>
-    </row>
-    <row r="43" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="15"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="24"/>
-    </row>
-    <row r="44" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="13"/>
-      <c r="C44" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="22">
+      <c r="D44" s="18">
         <f t="shared" ref="D44:I44" si="0">SUM(D13:D43)</f>
-        <v>176.5</v>
-      </c>
-      <c r="E44" s="22">
+        <v>0</v>
+      </c>
+      <c r="E44" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F44" s="22">
+      <c r="F44" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G44" s="22">
+      <c r="G44" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H44" s="22">
+      <c r="H44" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I44" s="22">
+      <c r="I44" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1477,30 +1312,28 @@
       </c>
     </row>
     <row r="47" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="29" t="s">
+      <c r="B47" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="30"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="33"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="27"/>
     </row>
     <row r="48" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="31" t="s">
+      <c r="B48" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="30"/>
-      <c r="D48" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="34"/>
-      <c r="H48" s="34"/>
-      <c r="I48" s="30"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="28"/>
+      <c r="H48" s="28"/>
+      <c r="I48" s="24"/>
     </row>
     <row r="49" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
@@ -1508,28 +1341,28 @@
       </c>
     </row>
     <row r="50" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C50" s="30"/>
-      <c r="D50" s="35"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="34"/>
-      <c r="H50" s="34"/>
-      <c r="I50" s="30"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="24"/>
     </row>
     <row r="51" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="31" t="s">
+      <c r="B51" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="30"/>
-      <c r="D51" s="35"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="34"/>
-      <c r="H51" s="34"/>
-      <c r="I51" s="30"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1816,15 +1649,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="ffcdf2b0-1459-4444-989c-847f95dff766" xsi:nil="true"/>
@@ -1841,6 +1665,15 @@
     </pngk>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1863,14 +1696,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93024C3E-FFB3-4472-BB22-2F4F8B37FD9F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E15A3931-78BE-46EE-8F26-4834832F54C2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1879,4 +1704,12 @@
     <ds:schemaRef ds:uri="e38bb144-3974-45f8-bb47-26071287cfd2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93024C3E-FFB3-4472-BB22-2F4F8B37FD9F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>